<commit_message>
changes done in sample user excel data
</commit_message>
<xml_diff>
--- a/sample_user -valid.xlsx
+++ b/sample_user -valid.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
   <si>
     <t>Role ID</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>07588775687</t>
+  </si>
+  <si>
+    <t>Rani</t>
+  </si>
+  <si>
+    <t>21/03/1978</t>
+  </si>
+  <si>
+    <t>testerindusnet@yahoo.com</t>
+  </si>
+  <si>
+    <t>07534775688</t>
   </si>
 </sst>
 </file>
@@ -204,10 +216,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -239,14 +251,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,12 +281,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -285,7 +312,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,47 +356,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -360,15 +378,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -389,55 +401,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,121 +569,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,6 +600,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,6 +654,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -645,39 +686,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -695,140 +707,141 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
@@ -1179,10 +1192,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1235,7 +1248,7 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1258,13 +1271,13 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H3" t="s">
@@ -1284,13 +1297,13 @@
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H4" t="s">
@@ -1310,7 +1323,7 @@
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="3"/>
@@ -1331,13 +1344,13 @@
       <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H6" t="s">
@@ -1357,13 +1370,13 @@
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H7" t="s">
@@ -1383,7 +1396,7 @@
       <c r="F8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1400,7 +1413,7 @@
       <c r="F9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1417,7 +1430,7 @@
       <c r="F10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1438,7 +1451,7 @@
       <c r="F11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="6" t="s">
         <v>49</v>
       </c>
       <c r="H11" t="s">
@@ -1484,7 +1497,7 @@
       <c r="F13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="6" t="s">
         <v>57</v>
       </c>
       <c r="H13" t="s">
@@ -1507,11 +1520,31 @@
       <c r="F14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="6" t="s">
         <v>60</v>
       </c>
       <c r="H14" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1529,6 +1562,7 @@
     <hyperlink ref="F12" r:id="rId10" display="sourav.basak@indusnet.co.in"/>
     <hyperlink ref="F13" r:id="rId11" display="sourav.basak@indusnet.co.uk" tooltip="mailto:sourav.basak@indusnet.co.uk"/>
     <hyperlink ref="F14" r:id="rId12" display="sourav.basak@talash.net"/>
+    <hyperlink ref="F15" r:id="rId13" display="testerindusnet@yahoo.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>